<commit_message>
Changed AbstractBase class to avoid out of service instances. Added dependency test to container
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProjectContainerTestData.xlsx
+++ b/src/test/test-data/ProjectContainerTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Project - Owner" sheetId="1" r:id="rId1"/>
@@ -1455,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3113,8 +3113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L41" sqref="L2:L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fixed container (Project) related test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProjectContainerTestData.xlsx
+++ b/src/test/test-data/ProjectContainerTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UC196992\Git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -964,24 +969,12 @@
     <t>hits[0].id||hits[1].id||hits[2].id</t>
   </si>
   <si>
-    <t>hits[0]._id</t>
-  </si>
-  <si>
     <t>{ "items" : [ {"id": "(OPQA-896_hits[0].id)", "type": "wos"}] }</t>
   </si>
   <si>
-    <t>status=200||(OPQA-896_hits[0].id).itemExists=false||(OPQA-896_hits[0].id).numberTotalContainers=2</t>
-  </si>
-  <si>
-    <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=2</t>
-  </si>
-  <si>
     <t>{"items" : [{"id": "(OPQA-896_hits[0].id)", "type": "wos"}, {"id": "(OPQA-896_hits[1].id)", "type": "wos"}, {"id": "(OPQA-898_hits[0].id)", "type": "patents"}, {"id": "(OPQA-898_hits[1].id)", "type": "patents"}, {"id": "(OPQA-897_hits[0].id)", "type": "posts"}, {"id": "(OPQA-897_hits[1].id)", "type": "posts"} ] }</t>
   </si>
   <si>
-    <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=2||(OPQA-896_hits[1].id).itemExists=true||(OPQA-896_hits[1].id).numberTotalContainers=2||(OPQA-896_hits[0].id).itemExists=true||(OPQA-897_hits[0].id).numberTotalContainers=2||(OPQA-896_hits[1].id).itemExists=true||(OPQA-897_hits[1].id).numberTotalContainers=2||(OPQA-898_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=2||(OPQA-898_hits[1].id).itemExists=true||(OPQA-896_hits[1].id).numberTotalContainers=2</t>
-  </si>
-  <si>
     <t>{"documents":[{"docType":"file","id":"0B175X3HOM71HZm01eEM0dWRoMHM","name":"RCCStories_for QA.docx","parent":"item","parentId":"(OPQA-896_hits[0].id)","parentType":"wos","url":"https://drive.google.com/file/d/0B175X3HOM71HZm01eEM0dWRoMHM/view?usp=drive_web"}]}</t>
   </si>
   <si>
@@ -1037,13 +1030,25 @@
   </si>
   <si>
     <t>1PSEARCHV4</t>
+  </si>
+  <si>
+    <t>status=200||(OPQA-896_hits[0].id).itemExists=false||(OPQA-896_hits[0].id).numberTotalContainers=3</t>
+  </si>
+  <si>
+    <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=3</t>
+  </si>
+  <si>
+    <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=3||(OPQA-896_hits[1].id).itemExists=true||(OPQA-896_hits[1].id).numberTotalContainers=3||(OPQA-896_hits[0].id).itemExists=true||(OPQA-897_hits[0].id).numberTotalContainers=3||(OPQA-896_hits[1].id).itemExists=true||(OPQA-897_hits[1].id).numberTotalContainers=3||(OPQA-898_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=3||(OPQA-898_hits[1].id).itemExists=true||(OPQA-896_hits[1].id).numberTotalContainers=3</t>
+  </si>
+  <si>
+    <t>hits[0].id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1165,6 +1170,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1211,7 +1224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1243,9 +1256,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1277,6 +1291,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1452,14 +1467,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="44.85546875" style="3" customWidth="1" collapsed="1"/>
@@ -1475,7 +1490,7 @@
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
@@ -1513,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="45">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1521,7 +1536,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
@@ -1543,7 +1558,7 @@
       </c>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="45">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -1551,7 +1566,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
@@ -1573,7 +1588,7 @@
       </c>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="45">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1581,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
@@ -1603,7 +1618,7 @@
       </c>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="15.75">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -1611,7 +1626,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>20</v>
@@ -1629,11 +1644,11 @@
         <v>13</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>315</v>
+        <v>339</v>
       </c>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="47.25">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>175</v>
       </c>
@@ -1663,7 +1678,7 @@
       <c r="K6" s="2"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="360">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>176</v>
       </c>
@@ -1695,7 +1710,7 @@
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="105">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>199</v>
       </c>
@@ -1727,7 +1742,7 @@
       </c>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="300">
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>209</v>
       </c>
@@ -1759,7 +1774,7 @@
       <c r="K9" s="2"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="105">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>210</v>
       </c>
@@ -1791,7 +1806,7 @@
       <c r="K10" s="2"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>211</v>
       </c>
@@ -1823,7 +1838,7 @@
       <c r="K11" s="2"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="375">
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>212</v>
       </c>
@@ -1855,7 +1870,7 @@
       <c r="K12" s="2"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="375">
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>213</v>
       </c>
@@ -1887,7 +1902,7 @@
       <c r="K13" s="2"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>214</v>
       </c>
@@ -1919,7 +1934,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="30">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>215</v>
       </c>
@@ -1949,7 +1964,7 @@
       <c r="K15" s="2"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>216</v>
       </c>
@@ -1983,7 +1998,7 @@
       </c>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" s="1" customFormat="1" ht="47.25">
+    <row r="17" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>220</v>
       </c>
@@ -2015,7 +2030,7 @@
       <c r="K17" s="2"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" ht="75">
+    <row r="18" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>221</v>
       </c>
@@ -2038,18 +2053,18 @@
         <v>76</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>179</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>222</v>
       </c>
@@ -2072,7 +2087,7 @@
         <v>79</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>179</v>
@@ -2083,7 +2098,7 @@
       <c r="K19" s="2"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="20" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>223</v>
       </c>
@@ -2106,7 +2121,7 @@
         <v>37</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>179</v>
@@ -2117,7 +2132,7 @@
       <c r="K20" s="2"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" ht="75">
+    <row r="21" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>224</v>
       </c>
@@ -2140,18 +2155,18 @@
         <v>76</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>222</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="22" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>225</v>
       </c>
@@ -2174,7 +2189,7 @@
         <v>79</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>181</v>
@@ -2185,7 +2200,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="23" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>226</v>
       </c>
@@ -2208,7 +2223,7 @@
         <v>79</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>203</v>
@@ -2219,7 +2234,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" s="1" customFormat="1" ht="375">
+    <row r="24" spans="1:12" s="1" customFormat="1" ht="375" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>227</v>
       </c>
@@ -2242,18 +2257,18 @@
         <v>76</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>203</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>320</v>
+        <v>338</v>
       </c>
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="25" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>228</v>
       </c>
@@ -2285,7 +2300,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" s="1" customFormat="1" ht="180">
+    <row r="26" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>229</v>
       </c>
@@ -2317,7 +2332,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" s="1" customFormat="1" ht="120">
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>231</v>
       </c>
@@ -2349,7 +2364,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" s="1" customFormat="1" ht="105">
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>232</v>
       </c>
@@ -2381,7 +2396,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="29" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>233</v>
       </c>
@@ -2413,7 +2428,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="30" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>234</v>
       </c>
@@ -2445,7 +2460,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="31" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>236</v>
       </c>
@@ -2466,7 +2481,7 @@
       </c>
       <c r="G31"/>
       <c r="H31" s="10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>222</v>
@@ -2477,7 +2492,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12" s="1" customFormat="1" ht="180">
+    <row r="32" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>237</v>
       </c>
@@ -2498,7 +2513,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>222</v>
@@ -2509,7 +2524,7 @@
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:12" s="1" customFormat="1" ht="120">
+    <row r="33" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>238</v>
       </c>
@@ -2530,7 +2545,7 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>236</v>
@@ -2541,7 +2556,7 @@
       <c r="K33"/>
       <c r="L33"/>
     </row>
-    <row r="34" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="34" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>239</v>
       </c>
@@ -2562,7 +2577,7 @@
       </c>
       <c r="G34"/>
       <c r="H34" s="10" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>238</v>
@@ -2573,7 +2588,7 @@
       <c r="K34"/>
       <c r="L34"/>
     </row>
-    <row r="35" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="35" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>240</v>
       </c>
@@ -2584,7 +2599,7 @@
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>1</v>
@@ -2605,7 +2620,7 @@
       <c r="K35" s="7"/>
       <c r="L35"/>
     </row>
-    <row r="36" spans="1:12" s="1" customFormat="1" ht="75">
+    <row r="36" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>241</v>
       </c>
@@ -2637,7 +2652,7 @@
       <c r="K36"/>
       <c r="L36"/>
     </row>
-    <row r="37" spans="1:12" s="1" customFormat="1" ht="120">
+    <row r="37" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>242</v>
       </c>
@@ -2667,7 +2682,7 @@
       <c r="K37"/>
       <c r="L37"/>
     </row>
-    <row r="38" spans="1:12" s="1" customFormat="1" ht="60">
+    <row r="38" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>243</v>
       </c>
@@ -2695,7 +2710,7 @@
       <c r="K38"/>
       <c r="L38"/>
     </row>
-    <row r="39" spans="1:12" s="1" customFormat="1" ht="45">
+    <row r="39" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>244</v>
       </c>
@@ -2718,12 +2733,12 @@
         <v>225</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="K39"/>
       <c r="L39"/>
     </row>
-    <row r="40" spans="1:12" s="1" customFormat="1" ht="180">
+    <row r="40" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>245</v>
       </c>
@@ -2750,12 +2765,12 @@
         <v>225</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="K40"/>
       <c r="L40"/>
     </row>
-    <row r="41" spans="1:12" s="1" customFormat="1" ht="90">
+    <row r="41" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>246</v>
       </c>
@@ -2782,12 +2797,12 @@
         <v>225</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K41"/>
       <c r="L41"/>
     </row>
-    <row r="42" spans="1:12" s="1" customFormat="1" ht="75">
+    <row r="42" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>247</v>
       </c>
@@ -2819,7 +2834,7 @@
       <c r="K42"/>
       <c r="L42"/>
     </row>
-    <row r="43" spans="1:12" s="1" customFormat="1" ht="30">
+    <row r="43" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>248</v>
       </c>
@@ -2830,7 +2845,7 @@
         <v>34</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>25</v>
@@ -2851,7 +2866,7 @@
       <c r="K43"/>
       <c r="L43"/>
     </row>
-    <row r="44" spans="1:12" s="1" customFormat="1" ht="45">
+    <row r="44" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>256</v>
       </c>
@@ -2862,7 +2877,7 @@
         <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>25</v>
@@ -2883,7 +2898,7 @@
       <c r="K44"/>
       <c r="L44"/>
     </row>
-    <row r="45" spans="1:12" s="1" customFormat="1" ht="30">
+    <row r="45" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>249</v>
       </c>
@@ -2894,7 +2909,7 @@
         <v>34</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>25</v>
@@ -2915,7 +2930,7 @@
       <c r="K45"/>
       <c r="L45"/>
     </row>
-    <row r="46" spans="1:12" ht="75">
+    <row r="46" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>250</v>
       </c>
@@ -2938,17 +2953,17 @@
         <v>76</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>248</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:12" ht="75">
+    <row r="47" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>251</v>
       </c>
@@ -2971,17 +2986,17 @@
         <v>95</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>248</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:12" ht="30">
+    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>252</v>
       </c>
@@ -3010,7 +3025,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="45">
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>254</v>
       </c>
@@ -3039,7 +3054,7 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="30">
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>253</v>
       </c>
@@ -3068,7 +3083,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="30">
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>255</v>
       </c>
@@ -3110,14 +3125,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L41" sqref="L2:L41"/>
+      <selection activeCell="L2" sqref="L2:L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" style="3" customWidth="1" collapsed="1"/>
@@ -3133,7 +3148,7 @@
     <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
@@ -3171,7 +3186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="409.5">
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>189</v>
       </c>
@@ -3202,7 +3217,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45">
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>257</v>
       </c>
@@ -3229,7 +3244,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="75">
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>258</v>
       </c>
@@ -3262,7 +3277,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="105">
+    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>266</v>
       </c>
@@ -3293,7 +3308,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="75">
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>267</v>
       </c>
@@ -3326,7 +3341,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="75">
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>270</v>
       </c>
@@ -3359,7 +3374,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="120">
+    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>271</v>
       </c>
@@ -3388,7 +3403,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="60">
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>272</v>
       </c>
@@ -3417,7 +3432,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="45">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>273</v>
       </c>
@@ -3446,7 +3461,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="105">
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>276</v>
       </c>
@@ -3475,7 +3490,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="60">
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>277</v>
       </c>
@@ -3504,7 +3519,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="45">
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>278</v>
       </c>
@@ -3533,7 +3548,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="45">
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>279</v>
       </c>
@@ -3562,7 +3577,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="75">
+    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>280</v>
       </c>
@@ -3591,7 +3606,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="75">
+    <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>281</v>
       </c>
@@ -3622,7 +3637,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="75">
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>282</v>
       </c>
@@ -3645,17 +3660,17 @@
         <v>76</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>274</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="75">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>283</v>
       </c>
@@ -3678,7 +3693,7 @@
         <v>79</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>274</v>
@@ -3688,7 +3703,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="75">
+    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>284</v>
       </c>
@@ -3711,17 +3726,17 @@
         <v>76</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>283</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="75">
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>285</v>
       </c>
@@ -3744,7 +3759,7 @@
         <v>79</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>275</v>
@@ -3754,7 +3769,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="195">
+    <row r="21" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>287</v>
       </c>
@@ -3777,17 +3792,17 @@
         <v>76</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>275</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="135">
+    <row r="22" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>288</v>
       </c>
@@ -3818,7 +3833,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="255">
+    <row r="23" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>289</v>
       </c>
@@ -3849,7 +3864,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="135">
+    <row r="24" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>291</v>
       </c>
@@ -3880,7 +3895,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="135">
+    <row r="25" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>292</v>
       </c>
@@ -3911,7 +3926,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="120">
+    <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>293</v>
       </c>
@@ -3942,7 +3957,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="120">
+    <row r="27" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>294</v>
       </c>
@@ -3963,7 +3978,7 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="10" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>283</v>
@@ -3973,7 +3988,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="225">
+    <row r="28" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>295</v>
       </c>
@@ -3994,7 +4009,7 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="10" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>285</v>
@@ -4004,7 +4019,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="120">
+    <row r="29" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>296</v>
       </c>
@@ -4025,7 +4040,7 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>294</v>
@@ -4035,7 +4050,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="105">
+    <row r="30" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>297</v>
       </c>
@@ -4056,7 +4071,7 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="10" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>296</v>
@@ -4066,7 +4081,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="105">
+    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>298</v>
       </c>
@@ -4097,7 +4112,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="60">
+    <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>299</v>
       </c>
@@ -4128,7 +4143,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="135">
+    <row r="33" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>300</v>
       </c>
@@ -4157,7 +4172,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="180">
+    <row r="34" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>301</v>
       </c>
@@ -4184,11 +4199,11 @@
         <v>285</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="90">
+    <row r="35" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>302</v>
       </c>
@@ -4215,11 +4230,11 @@
         <v>285</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="60">
+    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>303</v>
       </c>
@@ -4230,7 +4245,7 @@
         <v>34</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>25</v>
@@ -4250,7 +4265,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="75">
+    <row r="37" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>304</v>
       </c>
@@ -4273,17 +4288,17 @@
         <v>76</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>303</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="90">
+    <row r="38" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>305</v>
       </c>
@@ -4306,17 +4321,17 @@
         <v>95</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>303</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="60">
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>306</v>
       </c>
@@ -4345,7 +4360,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="45">
+    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>307</v>
       </c>
@@ -4376,7 +4391,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="45">
+    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>308</v>
       </c>

</xml_diff>

<commit_message>
Fixed container - project test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProjectContainerTestData.xlsx
+++ b/src/test/test-data/ProjectContainerTestData.xlsx
@@ -189,9 +189,6 @@
     "imgtype": "png" }</t>
   </si>
   <si>
-    <t>status=200||type=project||name=Project about cancer created From API||desc=Cancer is a group of diseases involving abnormal cell growth with the potential to invade or spread to other parts of the body.[1][2] Not all tumors are cancerous; benign tumors do not spread to other parts of the body.[2] Possible signs and symptoms include a lump, abnormal bleeding, prolonged cough, unexplained weight loss and a change in bowel movements.[3] While these symptoms may indicate cancer, they may have other causes.[3] Over 100 cancers affect humans.||userid=(SYS_USER1)||ispublic=false||isOwner=false</t>
-  </si>
-  <si>
     <t>Verify that user is able to create multiple projects using container API</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>status=200||type=project||name=Project1 about cancer updated title from API||desc=Cancer is a group of diseases involving abnormal cell growth with the potential to invade or spread to other parts of the body.[1][2] Not all tumors are cancerous; benign tumors do not spread to other parts of the body.[2] Possible signs and symptoms include a lump, abnormal bleeding, prolonged cough, unexplained weight loss and a change in bowel movements.[3] While these symptoms may indicate cancer, they may have other causes.[3] Over 100 cancers affect humans.||userid=(SYS_USER1)||isOwner=false||ispublic=false</t>
   </si>
   <si>
-    <t>status=200||type=project||name=Project2 from API about multiple projects test||desc=API test for creation of multiple projects for the same user.||userid=(SYS_USER1)||isOwner=false||ispublic=false</t>
-  </si>
-  <si>
     <t>Verify that project owner is able to add project cover photo to exisintg project using container API</t>
   </si>
   <si>
@@ -318,9 +312,6 @@
     <t>{ "name": "Project3 about testing invitations From API", "desc": "This project is about to invite new members into the project and testing member permissions like adding items, documents to the project etc..", "type": "project", "image": "data:image/jpeg;base64,/9j/4AAQSkZJRgABAQEASABIAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wAARCAD6APoDASIAAhEBAxEB/8QAHAAAAQUBAQEAAAAAAAAAAAAAAAIDBAUGBwEI/8QAPRAAAQMDAgQDBgMGBgIDAAAAAQACAwQFEQYhEjFBURNhcQcUIoGRoTKxwRUjQlJi4TNDU3LR8QglssLi/8QAGwEBAAEFAQAAAAAAAAAAAAAAAAMCBAUGBwH/xAAwEQACAQMDAgUDAwQDAAAAAAAAAQIDBBEFITESQQYTIlGBMmFxobHBFJHR4QcV8P/aAAwDAQACEQMRAD8A+qUIQgBCEIAQhCAEIQgBCEIAQhCAEIQgBCM45poTtP4cu9AgHUJtkrHnAO/bqnEAIQhACEIQAhCEAIQhACEIQAhCEAIQhACEIQAhCEAIQhACEIQAhCEAIQhACEIQFTcqkGtipAcAt43+YzsPzVnHw8A4cYwsbq6c22901UdoZ4/D4ugc08vofspEF9YY/wAaAt71IImeJE7hkZuCFNt9SKujhqG8pGg47HqsHf7+xsD/AIt1stN08lNYqKGYESiMF4PQncj7oCzQhCAEIQgBCEIAQhCAEIQgBCEIAQhCAEIQgBCEIAQhCAEIQgBCEIAQhCAExVzsp4HSSHYbDzJ5J9ZT2g1Hh22GHJHG8uJHZo/uEA1qOd1zt8lLPDC+F/TfLT0IPQjuua1NtvNK/gpp45GdPEyCPoriyXKtZbKOWvxwVTHSQu7tDy0Z89gfmFYisY94JwgIejaCnhuLai/mWWojdxRANzCw9CRzJH0XWIZY5ow+J4ew8iDlYKGppmAOfgKxtt7pG1EIpJg7jkax7Ry3OEBsUIQgBCEIAQhCAEIQgBCEIAQhCAEIQgBCEIAUerqG07W9XuOGt7lSFnbxVCK907JD8Ii4h653QF2yN7m5lecnoNgFHq3zUo8RhL2DctcnYKtjowSVButawROGUBZUk8dTA2WI5Y77eSeWa0XUmeCuaN2MnwPm0ErSoAQhCAEIRlACwHtNmcI3EAlsUDj8z/0t6Xt7hYPXQFVWxUOcGqmhgOOgcd/sSmQQtT20Uvs7sszBh1DHCHeQeAD9yFj46twaDldE9r9W2k0HWNwB4r4om+Xxh35NXDIbziIYccDYrxtLk8bS5LrU10nFAYadxEspEbcc8nZbesoI7JfnUkADY4hA8Y5fhAP1LSfmuUe9vq7jSOByI5Wv+hBXZ9asdNqSqMY/BTRgnzJdhenp0kckJDM8DcjfAyloAQhCAEIQgBCEIAQhCAEIQgBCEIAQhCAFnNX2uespmVNBvWU2S1n+o082+u2y0aQ9wa0ucQGgZJPRAcrg1Q2MuimLo5W7OY8cLgfMFQLlqY1DhBS5lnfs1jdySrvU8EV+uHi1FNG+Fnwx8TRnHf5qlZb6a1yE08bI8/yjCA1+gallKDapS01b2mpc4dTkAj5bfRbZcNsl6FNrmGZzsRs4WvP9Lsg/nn5LuQQAheZXhKA9KyvtDu09o08+aleI5pHtia/qM55eey0+VzX/AMgXcPs6nkBwWVMLs9viVvc58mXS8PDILlN0pdLw8HNpqmolmM0k8zpc5L3POc+q0WkrrUXDVtlgr5nSCF75C+U9GxnGT5Llmmqi71tRG8uk9yb+J8vJw7DPNa0tWn0LqdjV6vq91n9zUaNzOxq9Wer3WTee12+0F2oIbXRziZ7JvEkdHu0YBGM9Tv0XMW0jWMDWNAaOiseFRbjUNoqKapkblsbc47ry5v611JZ+Eim5v6t1JZ+ENU1GyOqifksaHAuA5YyuxaemGotT1dVEeKl94MvFjmxmGsHzIz6ZXzi7VdS55LXRsB6Bo/VfQHsvulJZfZ1QXa6TOEle92C1pc44c4AYHoSs5plxVgnGvL0pZy+3yZzTa9aClGvL0pZy+3ydUJ8koHIVZaLvR3WnE9DM2RmcHHMHsR0VgHLNxkppSi8ozMZKa6ovKHELwFegqoqBCEIAQgnAUYVLXkiIOkx1byQElCY8doOHhzP93JPhACEIQAhCEAIQhACgXU8ULIeIDxXcJ8xzKnqg1iXR2+CVmQ5kzd/UEICqvs1NRANLmh3ZYG93APf8JVBrKqqTqeJ3iv4AzcZ2O6i3CsDIuN7hsMoDUHTErbNQ6lgY6VjmvFXENzwBxDXjuAM58sHuun6QvEVwoWRCQOexo4TnPE3+y90JLHLomxPiOWvooj8y0Z++Vj9T2yfStxbc7Tllukky5jRtA8//AFP25dQgOml2AotbX01GziqZ2RD+o7n0Cw1115B+y6YxStpquZxY/i/hwM5HrnZUMdU2tJlbOJz1dxcRWA1XWv6OXlQhmXu+DJWenf1EeuUsL9TX3rWkdJSTS0NK+pcwZ+I8Ix1PU7c1zrUGp7jf4HU9a6L3R5BMDGDgODkZzknfBV2FmrrbjRyOkgaTSu3wB/hnt6du3LstblrFxc5jUlhey2Ri/EulVoUVUtW+lfUv5/0V+OiMKws9E2snd4vEYmDJx1PbKvJLVRPZwmBrexbsR81Zzrxi8M13TvDNzfUfPTUU+M53/wAGTwm6injqYJIZmB8TwWuaeoUmePwaqeEu4jE/h4u+wP13ScKVPujAVqU7erKnLaUXh/lGEqtBZmJpK8tiJ2bIzJHzB3W6o5J4NPW20Pm8SmoWuEfw4yXHJJ+q9UaurKehh8WqlbG07DPMnyHVXUrqtUj5bec/qTxrXFxijDMm9sJbv7bLLLrT94qLJcWVVKcjlJGTgSN7H9Cu3Wq4wXKhiq6V3FHKMjuD1B8wvlCv1c5xLaCAAcg+Xc/Qf8rReyn2iT2W9mlvdS59srHAFzuUL+jgByHQ/I9Fm9IlWoPoqfS/0Z0HRvCGs0redatDphjKi3v8JZ/sfTYelNcocUge0EEEEZBB5hN11xpbbTOqa+phpoG/ikleGtHzK2XOCNRcn0pblkD2SgVmbXrLT11qRBbrzRzznYRtkHEfQHn8lomvyMheKSlwyqpSqUn01ItP7pr9ysvNSRNBSNOPEy5/oOnzVnTta2JoaABhZPV8xorrQ1LsiORhiz/UDkD6E/RTqK8MMY+IL0oLytDTC7iVfZasyungccuhIIP9J/6Vdcbw0Ru+IJjQ8jquruNX/lZbE09yMk/mEBr0IQgBCEIAQhCAFUapZ4liqh1aA/6EFWpKYqGMmifFKOKN4LXDuCgPn/WFI51wErRyYufXyslmeKaM4ceZ7Bd81P4NnmFJWwNrKKRnG1xAD27kEeeNt9ua55XUdhpzHW22FlQzxy8h5PE04A4fQbHHTKhuK3kUpVGs4WSSlT82agnjJsNE6mmt+gbXQshd75Ex0eZBs1vEeE467EJMtfV1c3FWTSzseQ18Zdhrmk7jHLllV9vqoK2PigfuPxNPMKc1nkuf3erXFer1TeEnsllL/ZtVKyo0odKWW+/c5t7Snz2yobRv50lQWcQ/iaWnhd6EYKb9mktbVXp8rA/3NkbhK8/hJPIeZyui1lso64g1tLDOQAMyN4th0UqCGKCJsUEbIo28msaAB8gpb/VoXSbjDDaw8kFvayoelyyhYSgEAL0LAl7kiV05o6KaaOMPLBnhG3qf1VM+9VTmkNETc/xBuf1WlOMKkr7KMl9FhveI7D5dvT8lNRlDiaNc12jqDgp2EsY5isZf3W3JR8y5xJLnEuJPMk9Ul7mxsLnuDWtGSXHAATdxqorbC+WtJiDObXD4iewHUrnt8vU90kLTmOmB+GIH7nuVlre2lWe3Huah4f8ACl9r9xJYcYp+qUk9n7b8s20F7t9RVNp4agOkccDAOD6FQ7/YDdahs7akxuawN4CMjn07LD0NQaSshqA3i8N4dg9cFdAg1DbJog81TIiebZPhI/5+SuK1vO3mpUs/ubFrfhq98K3lK50nqmsP1YTw+6wk+VwYa72motMrG1HCWvzwPachyrye60WrLzFcjDBSAmKJxcXuGOI4xsO3NZ3ORvzWVt5TlTTmsM694Zu7+80+FXUYdNR52xjK7Nrs2dW9m3tWksVPFbL62Wot8Y4YZmbyQj+Uj+Jv3Hmqz2x61ptW3Cijtb5jQUsZOXAtD5HHc8PkABnzK53kAlM1TXuhe2N3DIR8JV5503Dy29iR6LaUbl30IerfZcZffHuOB7mPDmvLXA5BBwR5r629kuov2/ou1y1NUJ64RcMjs7vLXEA+ZIAJXw7U1FSwujmc4OGxBJXdvZTUzW60UkMMkpqZI2mOGNpc/JHQDdXlpBxbZp3iq/hcwhFRw03zzxwfTN1t9PdqCSkq2F0T98jYtI5OB6ELk1cy5WuunpaV/vkMTuFso+An1B/RWMDtXsMbq1k0FM94bxSTNLt/6QSc+qtDa3RsDnD6q+NKMgx9xr52RVB92iLg1xzlxyei7RbKCC2UEVLRx+HDGMAdT3J7krlUmJtS2+lYf8SdgOP9y7EEAIQhACEIQAkkpRTTigBzky9y9c5MSOQGN9pMPiUlJLjkXRn0Iz+ixmm7U+56AvlFAI/eI6/xmF+3JjCRnpkArf61HiWVxPNkjXfp+qx+jak0lvvcbMcTqhgGf6mnP5K2vJQhQnKp9KTyS0FJ1I9HOTmbayainEkbnRyNOxC6LZKx1xtcFU6MsdINxjG+cZ9FMbTQNaGiGINHTgCp9T6hisZp2GPxZpslrc4AA5n7rm1aqrmXTSjv+uDa45isyZdgL3CqrDfKa8RnwcsmaMujJyfUdwrfCs5xlB9MluV5yZ3VeoDZ2xw08bZKqUcQ4vwsb3PdZFmrbw2TiNRG4fymJuFr9V6d/bHhTQSNjqYxw/EPhc3se391h7xYq20xskqmsMb3cIcx2d8Zx9l1vwXb+Hrm0jQuEpV5NpqXL32x8GpaxU1CnWc6baguMcfJ0XT10/a9sjqvD8N+Sx7c5AcO3knrtdKW1U3jVb8Z/CwbueewC5tadQ19qonUtIYvDLi9pezJaTzwq+sqp6yczVcr5ZTtxOPTsOyjpf8AG9WrqE3VajbqTxh5bXZfYrl4ijG3j0rM8b7YWf5HdR3CS/1HiVoAY3aKNp2jHkep81mKyifTguGZIueRzHr/AMq6Ud9fTscW8eSOZaMgfNb7e6DpdO1jQklTUdk8pNfPf5IdC1zVbe4crXqnneUcNp/C4/JRdNkcyl1Bj94kMDS2I4IBGN+u3ZI67Ll9zSVGrKkpKSTxlcP7o7vZ15XVCFWcHFySbi+V9hPJeFKIyVAu9Q6mp+JmxJxxdlFFZeCS4qxoU3UlwiW5ePKywqng5LiT3yrm01Jna5rzktxgquVNxWTF22qQuJ+XjDZLdHTunhkqaeOoEbg7gfkBwHQkEHBX0p7HtYabuuLZbLVHabr4Ze+JjeIStGMkP5kb8j918zVk8cDck5PRo5ldA/8AGESVftFuFS/lDb3+gy9gVzaykpYXBrniqjaypOUl61w1/J9MahnjgioZpv8ABZUtDj2y1zR9yFUa0v1PQUkLYPjfMeEY6KXrX4tJ3E9Y2CUerXArn+oz7za6SYHJa9p+qyZzgmaKcazXFE+TcN43fMMcQuzBcg9ntO5up6V4B2a9zvIcBH5kLrjSgHULwL0IAQhCADyUdzlIPIqG8oBL3bKPI7ZKkdhRZX4QFJq53/qJB3c381zSOWSO330xOLJI308wI6YcQuhaqk4qIRjm54+y5hLVilrLjFK34KmDgGRtxA5GfqVDcU/NpSp+6aJKU/LqRn7MedqeqZDvFCX4/Fg/kuf3iS46g1TTxx5mmLSTk8LWNH5BWDbpFI8QTZglO3x/hPoVs9I2ClpPFrfHbUVUzeAkfhY3OcD7b+S1fT9JnCr64YXv/gzd1e0/L9EssxVM24aeucTp4zHIDlpzlrvmF1ahr4au3sq2uayJzcuLjgNPUEqj1BQxyU5hm/wXnY9WO6ELnF1lmorlFQ1LnBuDhuTw8WdiB5jCvX4aV/eQoKfSpZ9TWeFnHb4Lb/tPJoSm45a7fk6v+22VVV7nZYJbnWH+CH8DfNzzsAvLn7OtT3zE9fWUMPDvHTNLnNZ88bnzW59mGnqey2SEBgNTI0Pmf1c4j8hyW4AwMLN2On2uj1uu1j1SjxKSy/ylwjG3FzWu4dNR4T7L+WfKmo9LXbTzsXKnAiJwJo3cTD8+nzVIvqrU9DT1lDNDURtfHI0tc0jmF8w3yhNsu9VRkkiN+Gnu3mPsujaNq7vs06qxNb7cNGBurbycOPBWVwkdRzNhz4hYQ3HPKzoII25LT5KZkpIJXl74mlx5kbZ9cKDxBoc9U6Jwn0uOVh5w8/g2Xwp4mp6I5wq0+qMsPKxlY/PYpaWHx6ljDnhO7sdlNrbcGtMlNnbcsO+fT/hWMMUcIxEwNHl1SlHZeF7enauhcJSk984w17Yf2JNS8a3lxfRurZuEY7KOdn75XG5mR8Q25JEsTZYiyRoLHcwVYXeBtO/xwQ2N5+LO2Hf3/NU89wYzaMF7voFzrUdPqWFzKhLtw/ddmdZ0zWrbU7KNxnnZrnD7o0Flh05KaShuGnqdzZHtidUxVMrJskgZ3cW9eWFV690o7RGqpLfDUvmp5YRPBI7Z3CSRh2OoLSomnXy1uqbPGTzrIsNHL8YX0TrXQ1r1fUwVNa+eGqhaY2yREfE3OeFwI8z9UpQlUg88mo6peULK9hKknGOHnl79njOx8suY+pk4WgueepX037CGaes2nzBS/uLrKBJVS1BAdLj+U/yjt55Uqy6DtlojDKS30Eh6yy8Rd885V1BpSkE5nMgimIxmnjDcehOSrqlR6OeTW9T1OV3LEdo/q/yXl+r6ess1bRwOMsk8Lo2lo+EEjYk8seixckDmWaKlnc3xWkN2PMjqtPLYqKKjne+Sqlc2NzgXzHmB5YWAtzeC1Gd+XSeHkuJyTt3UxiTp3s+pOCCesc3AkxHGTzIHM+mfyWya5Uun4fdLLQwdWQtB9cZP3Vo16AltKW1R2uTzCgFoQhAB5FQHlTzyKgSckBGlKhVDsAqXMq+qJwUBnb9VsinpjLvHx4d81Dvtjp6qn4omNMbhnYKReaYVETmuGQVAst1NE73G4O/dnaOR3I+R80By2/WJ1DWeHK0ugkPwuI5eRT1qhuVvcHUE2Wf6b9x/ZdB1tDRi1zvnexreHLTn+LpjzVNYqdz6OJ8jcEgHBCAivFzuz4WVbY4IGOD3cBJL8dPIKl9ptoLqWju0LMmjcBMAObMjB+RH3W9ZEGjkrK2Wdt1ZOyYjwOHheCM8Wen0UtGp5VSM/YpnHri4+5ptJ3eKeggkjeCxzA4EdiFpvfY+HOVyqnsVRpaljhtj5qiljyAyR2XNGeQPUDslO1UWN4ZGStfywWHP5KOWMtrg9Wcbm2v1yYIXfEOS+c9X1bKvUNXIwgtBDc+gWu1bqG4Gic6npZ+E85C04aO56rmfiFxLick7k91tXhu2anK4fGML+TH39RNKCHgeyUCmgR3Uf9oUolbH4zeMnAxyz6rcHUjH6mYzDfBKnnjgiMkrg1oVNU3h8mRAOBvc7lWFyoG10bA6RzCwkggfovbBpSOvuTYKivEUZGRhnxPPYdArC9rVacXJL0ruuSSlFSaXcy1zldJTuMjiSSNzupentI3q/vb7hRvbAec83wRj5nn8srtdn0nZrbwmKiZNKN/FnHiOB8s7D5BaWM4AA2HZc71Scb2v5qzjGDcdL1Opp9s6EIrqbbz/AG7GS0L7O6DTs7K6rk99uTfwPIwyI/0jqfMrobJFBY5OhytYxUVhFpcXFS5n11XllgyTzToqAOqp6iq8GIu6BV1BXiujEvi7Hk0HkqiE0twqwLZWHP8Akv8A/iVg4W8Noa3u0BXd0m4bbUhpO8bhz7hVT4y23xjpkIDrFBMHUcB7xt/JTY35WfskxfbaU5/y2/kruA7ICfGVJjKhxlSouYQDyEIQAeRUGQKceRUOQICFKFBnZkFWMgUWVvNAUlVBxBUldbWTtLXtBB5grUTMyocsaAxh0xRmZskjHPLN2h7i4N9AeSsG0zY2gNGAFcSRqNIxAV7mKnuOoX6dnFTkmEOaJGjt3V/I1ZfVNglu8ZjimjjY8/EXAkj0HVAdChukVXA12xDhnKQ1kEr+Q3WStbHUNOyl8R8giaGh7ubhjmVZx1TmkHKA0cdogfvgHKyetfZpS11HLVWtjaeuaC7DdmyeRHQ+aspb2aSB0jnYa0ZJVdovXbtV0NwfTh8ccEroSHYy7HX5q5t7irQl103hr/25RUhGa6ZHzbdK+R7nRYMbWktLTzyO6qC97S2bgc5jHAk42591vhpWav1LcZ54iKUVj2sBGzzxdfJdCu9vbLp+uoqSCMB8D2RxNaAM8Jxt6rMXGrdU1jd7fhFjG1eMvY5xS1MVTGHwvDgenUKZbauOK9W+MOBkfURtAB5ZcFiaVrozwyNcx7Twua4YIPUFaPR1FNXanoRAwubDK2WR2NmtG+/0wtiuL9u2k2sbP9i0hT9aO2sT7E0wJ9gXPDODjEvOy8aEojZARK34o3A8lz66UlZb6h81snLA48Ridu0n06LZ3KZ3vUFODwmUkZ9ApTbDFOz4m8R9UBzmm1LXSTMo6uBw8VwZxNORut/K0CijDuWQq26aZZTyRzQxHLXt6+at66nD6Rkcgy0kZCA1GmpAbfAAdgFpYDlZaxsLGNAGwWpph8IQE6LkpcPMKJH0UqHmEA+hCEAHkorwpR5Jl4QEOQKNK1TZAo0jUBXyM2UWVisJG81FlagK6RiiStVlK1RZGc0BXSMUWRqsJGqLI1AQooPEqHf7QnH07go1ZcI7XURyTh3hPBaSBnGP+07SX+31j3NhnY5zeYzuEBnNbz+Banxl3D4hDSfLqpmgrHTWOpurKL4aeqImEfRhxggeXVQtZUv7RwGn92N/VWliqHQ0VPKGcZMLWEZwcjbK9y0sHmFyRm07m1Ernu4vjcWgDAbk/mnw1OhpJJcNySdksMXh6VFdp613Gbxqyhhkl6vALXH1IxlT7dbqWgh8Kip4oI+ZDG4yfPupjWJ1jFW6k3HpbePbJT0pPONxLGJ9jF61ifYxUFQlrErgKfYzyTojygM7e7aKuIYJZIw8THt5tPdVkF0utuPBPEKhg5PZ8LvpyK2pg4hyUeS3tfzagKAarhe0MqWyRE/6jCB9eSf99juT44qQtkcSD8G4A7nsrRtljPNgPyVpb7eynH7tgb6BATrfAGMbgK4gbhQ6VmAFPiCAkxhSYhuExGpMY5IBxCEIASHhLXhCAjvao0jVMeEw9qAgyNUaRqsHtUZ7UBXyMUSRqs5GKJIxAVkjVEkarOVmygzDAKAob/AJKLON2OB/T9VmNHwNF1vOWggtiBBH+9bC44dTSMPUYWStzjbr9WswXeNGDt/Sf/0gJzqQQVcse5YfiYCeQ7KVaW4pns/ke4fr+qYlrGTTxgtLX7jB6hSLceGeoaeRw79EBNDEtrEtgynmtQDTY08xidYxPMjQDTWJ9jEtrE+2NANsYn2RpxkafYxAMti6J5kHkn441IZGgGGQDsnmxY5KQ1idDEAzEzBUyNqQ1ikRhAKYFIjSGjZONGEApCEIAQhCAQ4bJp4T5SHBARHtTEjVMeEw9qAhSNUaRinPao8jUBWzMVbVNwCrmVuyrKxmxwgMpdJSHBo6lZ+5PFNf4JHbNeCw/MLRV8BdVsDhsScLO61h8Kk94fsIxxZ9EBHbUtqdUUVMw5DSXOx6FXtZKykrSSeFpbj6FYjQfiT6hhmlyXu4nn6LdXOkFTcKdrm53OB5oBdPcozjOcd8bK5pnCRoLdwU0+3w0lJ4k+BtyUawucYyd+Aklo7DOyAumMT7I0qFmQpLI0A2yNPMjTrI08yNANsjT7GJbI0+yNAIYzdPsYlMYn2MQCGtToYlNanGtQCA1ONalBvklgID1o2Sl4AvUAIQhACEIQAvCF6hANPamXtUohIc1AQZGKPIxWLmZTLo0BVSRlQp4M5V2+JMSReSAylxt5ljPDs9py12ORWK1Xaq65QtgmaxkLTl3CSeLyXVpafKg1FvEgIIQHK9IWr3W6SvcMcAAGfNa2sdBSyMnkc0lh4huptVpxz5C+CR0TzsSBnPqFGGl3F7XVU7pgDkNxhv06oCpkmqL3OHPDm0oOw/n/stBb6TgA2UymtzYhgNVjBTABANQw4HJSo4/JSGQp9sSAjsjTzY0+2NOtjQDDY08yNOtYnGsQDbWeSda1LaxOBqAQG4Sw1KwvUB5he4QhACEIQAhCEAIQhACEIQAhCEAktCSWJxeICO6PyTRiUtySUBDdCOyQ6EdlMdzSCgIToAm3U47Ke5IKAg+B5JbYcKSea9HNANtjTrY0oJxqASI0sMTjUsIBAYlBqV1XqAMIQhACEIQAhCEAIQhACEIQH/2Q==", "imgtype": "jpeg" }</t>
   </si>
   <si>
-    <t>status=200||type=project||name=Project3 about testing invitations From API||desc=This project is about to invite new members into the project and testing member permissions like adding items, documents to the project etc..||userid=(SYS_USER1)||ispublic=false||isOwner=false||imgtype=image/jpeg</t>
-  </si>
-  <si>
     <t>1PGROUPS</t>
   </si>
   <si>
@@ -1042,6 +1033,15 @@
   </si>
   <si>
     <t>hits[0].id</t>
+  </si>
+  <si>
+    <t>status=200||type=project||name=Project about cancer created From API||desc=Cancer is a group of diseases involving abnormal cell growth with the potential to invade or spread to other parts of the body.[1][2] Not all tumors are cancerous; benign tumors do not spread to other parts of the body.[2] Possible signs and symptoms include a lump, abnormal bleeding, prolonged cough, unexplained weight loss and a change in bowel movements.[3] While these symptoms may indicate cancer, they may have other causes.[3] Over 100 cancers affect humans.||userid=(SYS_USER1)||ispublic=false||isOwner=true</t>
+  </si>
+  <si>
+    <t>status=200||type=project||name=Project2 from API about multiple projects test||desc=API test for creation of multiple projects for the same user.||userid=(SYS_USER1)||isOwner=true||ispublic=false</t>
+  </si>
+  <si>
+    <t>status=200||type=project||name=Project3 about testing invitations From API||desc=This project is about to invite new members into the project and testing member permissions like adding items, documents to the project etc..||userid=(SYS_USER1)||ispublic=false||isOwner=true||imgtype=image/jpeg</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
@@ -1536,7 +1536,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
@@ -1554,7 +1554,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="L2"/>
     </row>
@@ -1566,7 +1566,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
@@ -1584,7 +1584,7 @@
         <v>13</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="L3"/>
     </row>
@@ -1596,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
@@ -1614,7 +1614,7 @@
         <v>13</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="L4"/>
     </row>
@@ -1626,7 +1626,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>20</v>
@@ -1644,13 +1644,13 @@
         <v>13</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="L5"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>53</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>52</v>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="I7"/>
       <c r="J7" s="2" t="s">
-        <v>55</v>
+        <v>337</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>36</v>
@@ -1712,10 +1712,10 @@
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>34</v>
@@ -1731,11 +1731,11 @@
       </c>
       <c r="G8"/>
       <c r="H8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8"/>
       <c r="J8" s="2" t="s">
-        <v>64</v>
+        <v>338</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>36</v>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>23</v>
@@ -1763,29 +1763,29 @@
       </c>
       <c r="G9"/>
       <c r="H9" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>23</v>
@@ -1795,29 +1795,29 @@
       </c>
       <c r="G10"/>
       <c r="H10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>23</v>
@@ -1827,10 +1827,10 @@
       </c>
       <c r="G11"/>
       <c r="H11" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>45</v>
@@ -1840,16 +1840,16 @@
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>23</v>
@@ -1859,29 +1859,29 @@
       </c>
       <c r="G12"/>
       <c r="H12" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12"/>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>23</v>
@@ -1891,29 +1891,29 @@
       </c>
       <c r="G13"/>
       <c r="H13" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
@@ -1926,26 +1926,26 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="K14"/>
       <c r="L14"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>1</v>
@@ -1956,26 +1956,26 @@
       <c r="G15"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>23</v>
@@ -1988,22 +1988,22 @@
         <v>40</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L16"/>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>48</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>34</v>
@@ -2050,32 +2050,32 @@
         <v>22</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18"/>
     </row>
     <row r="19" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>21</v>
@@ -2084,13 +2084,13 @@
         <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>43</v>
@@ -2100,16 +2100,16 @@
     </row>
     <row r="20" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>21</v>
@@ -2121,10 +2121,10 @@
         <v>37</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>45</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="21" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>34</v>
@@ -2152,32 +2152,32 @@
         <v>22</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>21</v>
@@ -2186,13 +2186,13 @@
         <v>22</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>43</v>
@@ -2202,16 +2202,16 @@
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>21</v>
@@ -2220,13 +2220,13 @@
         <v>22</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>43</v>
@@ -2236,10 +2236,10 @@
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" ht="375" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>34</v>
@@ -2254,32 +2254,32 @@
         <v>22</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="K24"/>
       <c r="L24"/>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>21</v>
@@ -2289,10 +2289,10 @@
       </c>
       <c r="G25"/>
       <c r="H25" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>43</v>
@@ -2302,16 +2302,16 @@
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>21</v>
@@ -2321,10 +2321,10 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>43</v>
@@ -2334,16 +2334,16 @@
     </row>
     <row r="27" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>1</v>
@@ -2352,30 +2352,30 @@
         <v>24</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K27"/>
       <c r="L27"/>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>21</v>
@@ -2385,10 +2385,10 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>43</v>
@@ -2398,29 +2398,29 @@
     </row>
     <row r="29" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G29"/>
       <c r="H29" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>45</v>
@@ -2430,16 +2430,16 @@
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>23</v>
@@ -2449,10 +2449,10 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>43</v>
@@ -2462,16 +2462,16 @@
     </row>
     <row r="31" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>21</v>
@@ -2481,10 +2481,10 @@
       </c>
       <c r="G31"/>
       <c r="H31" s="10" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>43</v>
@@ -2494,16 +2494,16 @@
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>21</v>
@@ -2513,10 +2513,10 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="10" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>43</v>
@@ -2526,16 +2526,16 @@
     </row>
     <row r="33" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>21</v>
@@ -2545,10 +2545,10 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>43</v>
@@ -2558,16 +2558,16 @@
     </row>
     <row r="34" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>23</v>
@@ -2577,10 +2577,10 @@
       </c>
       <c r="G34"/>
       <c r="H34" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>43</v>
@@ -2590,16 +2590,16 @@
     </row>
     <row r="35" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>1</v>
@@ -2608,24 +2608,24 @@
         <v>24</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K35" s="7"/>
       <c r="L35"/>
     </row>
     <row r="36" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>34</v>
@@ -2640,30 +2640,30 @@
         <v>24</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K36"/>
       <c r="L36"/>
     </row>
     <row r="37" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1</v>
@@ -2674,26 +2674,26 @@
       <c r="G37"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="K37"/>
       <c r="L37"/>
     </row>
     <row r="38" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>1</v>
@@ -2702,7 +2702,7 @@
       <c r="G38"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>47</v>
@@ -2712,16 +2712,16 @@
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>1</v>
@@ -2730,26 +2730,26 @@
       <c r="G39"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="K39"/>
       <c r="L39"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>1</v>
@@ -2762,26 +2762,26 @@
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="K40"/>
       <c r="L40"/>
     </row>
     <row r="41" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>1</v>
@@ -2794,26 +2794,26 @@
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K41"/>
       <c r="L41"/>
     </row>
     <row r="42" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>1</v>
@@ -2822,30 +2822,30 @@
         <v>24</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="K42"/>
       <c r="L42"/>
     </row>
     <row r="43" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>25</v>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>43</v>
@@ -2868,16 +2868,16 @@
     </row>
     <row r="44" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>25</v>
@@ -2890,7 +2890,7 @@
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>45</v>
@@ -2900,16 +2900,16 @@
     </row>
     <row r="45" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>25</v>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>43</v>
@@ -2932,10 +2932,10 @@
     </row>
     <row r="46" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>34</v>
@@ -2950,25 +2950,25 @@
         <v>22</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>34</v>
@@ -2983,31 +2983,31 @@
         <v>22</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>25</v>
@@ -3018,7 +3018,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>13</v>
@@ -3027,16 +3027,16 @@
     </row>
     <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>25</v>
@@ -3047,7 +3047,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>42</v>
@@ -3056,16 +3056,16 @@
     </row>
     <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>25</v>
@@ -3076,7 +3076,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>13</v>
@@ -3085,16 +3085,16 @@
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>25</v>
@@ -3105,7 +3105,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>42</v>
@@ -3188,7 +3188,7 @@
     </row>
     <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>52</v>
@@ -3207,11 +3207,11 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="2" t="s">
-        <v>98</v>
+        <v>339</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>36</v>
@@ -3219,43 +3219,43 @@
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>23</v>
@@ -3268,27 +3268,27 @@
         <v>40</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -3299,27 +3299,27 @@
       <c r="G5" s="1"/>
       <c r="H5" s="10"/>
       <c r="I5" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
@@ -3329,30 +3329,30 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>21</v>
@@ -3362,88 +3362,88 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>23</v>
@@ -3454,7 +3454,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>13</v>
@@ -3463,16 +3463,16 @@
     </row>
     <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
@@ -3483,25 +3483,25 @@
       <c r="G11" s="1"/>
       <c r="H11" s="10"/>
       <c r="I11" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>25</v>
@@ -3512,7 +3512,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>42</v>
@@ -3521,27 +3521,27 @@
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>13</v>
@@ -3550,27 +3550,27 @@
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>13</v>
@@ -3579,16 +3579,16 @@
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>1</v>
@@ -3599,25 +3599,25 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>23</v>
@@ -3627,10 +3627,10 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>45</v>
@@ -3639,10 +3639,10 @@
     </row>
     <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
@@ -3657,31 +3657,31 @@
         <v>44</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>21</v>
@@ -3690,13 +3690,13 @@
         <v>44</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>43</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>34</v>
@@ -3723,31 +3723,31 @@
         <v>44</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>21</v>
@@ -3756,13 +3756,13 @@
         <v>44</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>43</v>
@@ -3771,10 +3771,10 @@
     </row>
     <row r="21" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>34</v>
@@ -3789,31 +3789,31 @@
         <v>44</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>21</v>
@@ -3823,10 +3823,10 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>43</v>
@@ -3835,16 +3835,16 @@
     </row>
     <row r="23" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>21</v>
@@ -3854,10 +3854,10 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>43</v>
@@ -3866,16 +3866,16 @@
     </row>
     <row r="24" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>1</v>
@@ -3884,29 +3884,29 @@
         <v>46</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>21</v>
@@ -3916,10 +3916,10 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>43</v>
@@ -3928,16 +3928,16 @@
     </row>
     <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>23</v>
@@ -3947,10 +3947,10 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>43</v>
@@ -3959,16 +3959,16 @@
     </row>
     <row r="27" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>21</v>
@@ -3978,10 +3978,10 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="10" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>43</v>
@@ -3990,16 +3990,16 @@
     </row>
     <row r="28" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>21</v>
@@ -4009,10 +4009,10 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="10" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>43</v>
@@ -4021,16 +4021,16 @@
     </row>
     <row r="29" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>21</v>
@@ -4040,10 +4040,10 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="10" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>43</v>
@@ -4052,16 +4052,16 @@
     </row>
     <row r="30" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>23</v>
@@ -4071,10 +4071,10 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>43</v>
@@ -4083,16 +4083,16 @@
     </row>
     <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>23</v>
@@ -4102,10 +4102,10 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>43</v>
@@ -4114,10 +4114,10 @@
     </row>
     <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>34</v>
@@ -4132,29 +4132,29 @@
         <v>46</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>1</v>
@@ -4165,25 +4165,25 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>1</v>
@@ -4196,25 +4196,25 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
@@ -4227,25 +4227,25 @@
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>25</v>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>43</v>
@@ -4267,10 +4267,10 @@
     </row>
     <row r="37" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>34</v>
@@ -4285,25 +4285,25 @@
         <v>44</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>34</v>
@@ -4318,31 +4318,31 @@
         <v>44</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>25</v>
@@ -4353,7 +4353,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>42</v>
@@ -4362,16 +4362,16 @@
     </row>
     <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>25</v>
@@ -4380,11 +4380,11 @@
         <v>46</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>13</v>
@@ -4393,16 +4393,16 @@
     </row>
     <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>25</v>
@@ -4413,7 +4413,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
modified testcase in container data
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProjectContainerTestData.xlsx
+++ b/src/test/test-data/ProjectContainerTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project - Owner" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="324">
   <si>
     <t>API</t>
   </si>
@@ -978,12 +978,6 @@
     <t>status=200||type=project||name=Project3 about testing invitations From API||desc=This project is about to invite new members into the project and testing member permissions like adding items, documents to the project etc..||userid=(SYS_USER1)||ispublic=false||isOwner=true||imgtype=image/jpeg</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>DEPFAIL</t>
-  </si>
-  <si>
     <t>{"items" : [{"id": "(OPQA-896_hits[0].id)", "type": "wos"}, {"id": "(OPQA-896_hits[1].id)", "type": "wos"} ] }</t>
   </si>
   <si>
@@ -999,7 +993,7 @@
     <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[1].id).itemExists=true||(OPQA-896_hits[0].id).itemExists=true</t>
   </si>
   <si>
-    <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=3||(OPQA-896_hits[1].id).itemExists=true||(OPQA-896_hits[1].id).numberTotalContainers=3||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[1].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=3||(OPQA-896_hits[1].id).numberTotalContainers=9</t>
+    <t>status=200||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=3||(OPQA-896_hits[1].id).itemExists=true||(OPQA-896_hits[1].id).numberTotalContainers=3||(OPQA-896_hits[0].id).itemExists=true||(OPQA-896_hits[1].id).itemExists=true||(OPQA-896_hits[0].id).numberTotalContainers=3||(OPQA-896_hits[1].id).numberTotalContainers=3</t>
   </si>
 </sst>
 </file>
@@ -1425,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,9 +1505,7 @@
       <c r="K2" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="L2" t="s">
-        <v>318</v>
-      </c>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1543,9 +1535,7 @@
         <v>28</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" t="s">
-        <v>318</v>
-      </c>
+      <c r="L3"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1609,9 +1599,7 @@
       <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L5" t="s">
-        <v>318</v>
-      </c>
+      <c r="L5"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1643,9 +1631,7 @@
         <v>50</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" t="s">
-        <v>319</v>
-      </c>
+      <c r="L6"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1677,9 +1663,7 @@
         <v>82</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" t="s">
-        <v>319</v>
-      </c>
+      <c r="L7"/>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1711,9 +1695,7 @@
         <v>35</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" t="s">
-        <v>319</v>
-      </c>
+      <c r="L8"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1809,9 +1791,7 @@
         <v>293</v>
       </c>
       <c r="K11"/>
-      <c r="L11" t="s">
-        <v>319</v>
-      </c>
+      <c r="L11"/>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1841,9 +1821,7 @@
         <v>163</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" t="s">
-        <v>319</v>
-      </c>
+      <c r="L12"/>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1877,9 +1855,7 @@
       <c r="K13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L13" t="s">
-        <v>318</v>
-      </c>
+      <c r="L13"/>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1911,9 +1887,7 @@
         <v>38</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" t="s">
-        <v>318</v>
-      </c>
+      <c r="L14"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1947,9 +1921,7 @@
         <v>313</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" t="s">
-        <v>319</v>
-      </c>
+      <c r="L15"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1983,9 +1955,7 @@
         <v>33</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" t="s">
-        <v>319</v>
-      </c>
+      <c r="L16"/>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -2019,9 +1989,7 @@
         <v>35</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" t="s">
-        <v>319</v>
-      </c>
+      <c r="L17"/>
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -2055,9 +2023,7 @@
         <v>314</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" t="s">
-        <v>319</v>
-      </c>
+      <c r="L18"/>
     </row>
     <row r="19" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -2082,7 +2048,7 @@
         <v>65</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>164</v>
@@ -2091,9 +2057,7 @@
         <v>33</v>
       </c>
       <c r="K19"/>
-      <c r="L19" t="s">
-        <v>319</v>
-      </c>
+      <c r="L19"/>
     </row>
     <row r="20" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -2118,7 +2082,7 @@
         <v>65</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>191</v>
@@ -2127,9 +2091,7 @@
         <v>33</v>
       </c>
       <c r="K20"/>
-      <c r="L20" t="s">
-        <v>318</v>
-      </c>
+      <c r="L20"/>
     </row>
     <row r="21" spans="1:12" s="1" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2154,18 +2116,16 @@
         <v>62</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>191</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K21"/>
-      <c r="L21" t="s">
-        <v>319</v>
-      </c>
+      <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -2197,9 +2157,7 @@
         <v>33</v>
       </c>
       <c r="K22"/>
-      <c r="L22" t="s">
-        <v>319</v>
-      </c>
+      <c r="L22"/>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -2231,9 +2189,7 @@
         <v>33</v>
       </c>
       <c r="K23"/>
-      <c r="L23" t="s">
-        <v>319</v>
-      </c>
+      <c r="L23"/>
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -2265,9 +2221,7 @@
         <v>139</v>
       </c>
       <c r="K24"/>
-      <c r="L24" t="s">
-        <v>319</v>
-      </c>
+      <c r="L24"/>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -2299,9 +2253,7 @@
         <v>33</v>
       </c>
       <c r="K25"/>
-      <c r="L25" t="s">
-        <v>319</v>
-      </c>
+      <c r="L25"/>
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -2333,9 +2285,7 @@
         <v>35</v>
       </c>
       <c r="K26"/>
-      <c r="L26" t="s">
-        <v>319</v>
-      </c>
+      <c r="L26"/>
     </row>
     <row r="27" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -2367,9 +2317,7 @@
         <v>33</v>
       </c>
       <c r="K27"/>
-      <c r="L27" t="s">
-        <v>319</v>
-      </c>
+      <c r="L27"/>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -2401,9 +2349,7 @@
         <v>33</v>
       </c>
       <c r="K28"/>
-      <c r="L28" t="s">
-        <v>319</v>
-      </c>
+      <c r="L28"/>
     </row>
     <row r="29" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -2435,9 +2381,7 @@
         <v>33</v>
       </c>
       <c r="K29"/>
-      <c r="L29" t="s">
-        <v>319</v>
-      </c>
+      <c r="L29"/>
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -2469,9 +2413,7 @@
         <v>33</v>
       </c>
       <c r="K30"/>
-      <c r="L30" t="s">
-        <v>319</v>
-      </c>
+      <c r="L30"/>
     </row>
     <row r="31" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
@@ -2503,9 +2445,7 @@
         <v>33</v>
       </c>
       <c r="K31"/>
-      <c r="L31" t="s">
-        <v>319</v>
-      </c>
+      <c r="L31"/>
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -2537,9 +2477,7 @@
         <v>188</v>
       </c>
       <c r="K32" s="7"/>
-      <c r="L32" t="s">
-        <v>319</v>
-      </c>
+      <c r="L32"/>
     </row>
     <row r="33" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2571,9 +2509,7 @@
         <v>190</v>
       </c>
       <c r="K33"/>
-      <c r="L33" t="s">
-        <v>319</v>
-      </c>
+      <c r="L33"/>
     </row>
     <row r="34" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -2600,12 +2536,10 @@
         <v>218</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K34"/>
-      <c r="L34" t="s">
-        <v>319</v>
-      </c>
+      <c r="L34"/>
     </row>
     <row r="35" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2633,9 +2567,7 @@
         <v>37</v>
       </c>
       <c r="K35"/>
-      <c r="L35" t="s">
-        <v>319</v>
-      </c>
+      <c r="L35"/>
     </row>
     <row r="36" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -2663,9 +2595,7 @@
         <v>301</v>
       </c>
       <c r="K36"/>
-      <c r="L36" t="s">
-        <v>319</v>
-      </c>
+      <c r="L36"/>
     </row>
     <row r="37" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2694,12 +2624,10 @@
         <v>208</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K37"/>
-      <c r="L37" t="s">
-        <v>319</v>
-      </c>
+      <c r="L37"/>
     </row>
     <row r="38" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -2731,9 +2659,7 @@
         <v>302</v>
       </c>
       <c r="K38"/>
-      <c r="L38" t="s">
-        <v>319</v>
-      </c>
+      <c r="L38"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -2765,9 +2691,7 @@
         <v>202</v>
       </c>
       <c r="K39"/>
-      <c r="L39" t="s">
-        <v>318</v>
-      </c>
+      <c r="L39"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -2799,9 +2723,7 @@
         <v>33</v>
       </c>
       <c r="K40"/>
-      <c r="L40" t="s">
-        <v>319</v>
-      </c>
+      <c r="L40"/>
     </row>
     <row r="41" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -2833,9 +2755,7 @@
         <v>35</v>
       </c>
       <c r="K41"/>
-      <c r="L41" t="s">
-        <v>319</v>
-      </c>
+      <c r="L41"/>
     </row>
     <row r="42" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -2867,9 +2787,7 @@
         <v>33</v>
       </c>
       <c r="K42"/>
-      <c r="L42" t="s">
-        <v>318</v>
-      </c>
+      <c r="L42"/>
     </row>
     <row r="43" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -2903,9 +2821,6 @@
         <v>313</v>
       </c>
       <c r="K43" s="2"/>
-      <c r="L43" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="44" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -2939,9 +2854,6 @@
         <v>313</v>
       </c>
       <c r="K44" s="2"/>
-      <c r="L44" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -2971,9 +2883,6 @@
         <v>13</v>
       </c>
       <c r="K45" s="2"/>
-      <c r="L45" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="46" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -3003,9 +2912,6 @@
         <v>32</v>
       </c>
       <c r="K46" s="1"/>
-      <c r="L46" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -3064,9 +2970,6 @@
         <v>32</v>
       </c>
       <c r="K48" s="1"/>
-      <c r="L48" t="s">
-        <v>319</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3081,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3196,9 +3099,6 @@
         <v>88</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -3231,9 +3131,6 @@
       </c>
       <c r="K4" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="L4" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -3266,9 +3163,6 @@
       <c r="K5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L5" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -3302,9 +3196,6 @@
       <c r="K6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L6" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -3338,9 +3229,6 @@
       <c r="K7" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="L7" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -3370,9 +3258,6 @@
         <v>251</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -3402,9 +3287,6 @@
         <v>102</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -3434,9 +3316,6 @@
         <v>13</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3466,9 +3345,6 @@
         <v>245</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -3498,9 +3374,6 @@
         <v>32</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -3530,9 +3403,6 @@
         <v>13</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -3562,9 +3432,6 @@
         <v>13</v>
       </c>
       <c r="K14" s="1"/>
-      <c r="L14" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -3594,9 +3461,6 @@
         <v>247</v>
       </c>
       <c r="K15" s="1"/>
-      <c r="L15" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -3628,11 +3492,8 @@
         <v>35</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>264</v>
       </c>
@@ -3664,11 +3525,8 @@
         <v>305</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>265</v>
       </c>
@@ -3700,11 +3558,8 @@
         <v>33</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>266</v>
       </c>
@@ -3736,11 +3591,8 @@
         <v>306</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>267</v>
       </c>
@@ -3763,7 +3615,7 @@
         <v>65</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>257</v>
@@ -3772,11 +3624,8 @@
         <v>33</v>
       </c>
       <c r="K20" s="1"/>
-      <c r="L20" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>269</v>
       </c>
@@ -3799,20 +3648,17 @@
         <v>62</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>257</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K21" s="1"/>
-      <c r="L21" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>270</v>
       </c>
@@ -3842,11 +3688,8 @@
         <v>33</v>
       </c>
       <c r="K22" s="1"/>
-      <c r="L22" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>271</v>
       </c>
@@ -3876,11 +3719,8 @@
         <v>33</v>
       </c>
       <c r="K23" s="1"/>
-      <c r="L23" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>273</v>
       </c>
@@ -3910,11 +3750,8 @@
         <v>152</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>274</v>
       </c>
@@ -3944,11 +3781,8 @@
         <v>33</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>275</v>
       </c>
@@ -3978,11 +3812,8 @@
         <v>33</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>276</v>
       </c>
@@ -4012,11 +3843,8 @@
         <v>33</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="L27" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>277</v>
       </c>
@@ -4046,11 +3874,8 @@
         <v>33</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>278</v>
       </c>
@@ -4080,11 +3905,8 @@
         <v>33</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="L29" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>279</v>
       </c>
@@ -4114,11 +3936,8 @@
         <v>33</v>
       </c>
       <c r="K30" s="1"/>
-      <c r="L30" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>280</v>
       </c>
@@ -4148,11 +3967,8 @@
         <v>33</v>
       </c>
       <c r="K31" s="1"/>
-      <c r="L31" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>281</v>
       </c>
@@ -4182,11 +3998,8 @@
         <v>182</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="L32" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>282</v>
       </c>
@@ -4211,14 +4024,11 @@
         <v>267</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="L33" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>283</v>
       </c>
@@ -4245,14 +4055,11 @@
         <v>267</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="L34" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>284</v>
       </c>
@@ -4282,11 +4089,8 @@
         <v>302</v>
       </c>
       <c r="K35" s="1"/>
-      <c r="L35" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>285</v>
       </c>
@@ -4316,11 +4120,8 @@
         <v>33</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>286</v>
       </c>
@@ -4352,11 +4153,8 @@
         <v>305</v>
       </c>
       <c r="K37" s="1"/>
-      <c r="L37" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>287</v>
       </c>
@@ -4388,11 +4186,8 @@
         <v>305</v>
       </c>
       <c r="K38" s="1"/>
-      <c r="L38" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>288</v>
       </c>
@@ -4420,11 +4215,8 @@
         <v>32</v>
       </c>
       <c r="K39" s="1"/>
-      <c r="L39" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>289</v>
       </c>
@@ -4454,11 +4246,8 @@
         <v>13</v>
       </c>
       <c r="K40" s="1"/>
-      <c r="L40" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>290</v>
       </c>
@@ -4486,9 +4275,6 @@
         <v>13</v>
       </c>
       <c r="K41" s="1"/>
-      <c r="L41" t="s">
-        <v>319</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>